<commit_message>
modify excel for cmg add saegw35,36
</commit_message>
<xml_diff>
--- a/scripts/EPCCMGCutoverTemplate.xlsx
+++ b/scripts/EPCCMGCutoverTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>用户数</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +219,14 @@
   </si>
   <si>
     <t>show vm 1 virtual fp | match "Worker" context all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHSAEGW35BNK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHSAEGW36BNK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,7 +645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1083,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1407,7 +1415,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>23</v>
@@ -1425,334 +1433,374 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="4">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4">
         <v>43404.875</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="6">
-        <v>30.1</v>
-      </c>
-      <c r="C21" s="6">
-        <v>59.916666666666664</v>
-      </c>
-      <c r="D21" s="6">
-        <v>27.03125</v>
-      </c>
-      <c r="E21" s="7">
-        <v>4.182861328125</v>
-      </c>
-      <c r="F21" s="7">
-        <v>15.127197265625</v>
-      </c>
-      <c r="G21" s="7">
-        <v>19.31005859375</v>
-      </c>
-      <c r="H21" s="5">
-        <v>698573</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="6">
-        <v>26.425000000000001</v>
-      </c>
-      <c r="C22" s="6">
-        <v>45.75</v>
-      </c>
-      <c r="D22" s="6">
-        <v>28.90625</v>
-      </c>
-      <c r="E22" s="7">
-        <v>3.118896484375</v>
-      </c>
-      <c r="F22" s="7">
-        <v>13.86669921875</v>
-      </c>
-      <c r="G22" s="7">
-        <v>16.985595703125</v>
-      </c>
-      <c r="H22" s="5">
-        <v>630718</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" s="6">
-        <v>25.5</v>
+        <v>30.1</v>
       </c>
       <c r="C23" s="6">
-        <v>39.541666666666664</v>
+        <v>59.916666666666664</v>
       </c>
       <c r="D23" s="6">
-        <v>29.875</v>
+        <v>27.03125</v>
       </c>
       <c r="E23" s="7">
-        <v>4.00634765625</v>
+        <v>4.182861328125</v>
       </c>
       <c r="F23" s="7">
-        <v>12.248046875</v>
+        <v>15.127197265625</v>
       </c>
       <c r="G23" s="7">
-        <v>16.25439453125</v>
+        <v>19.31005859375</v>
       </c>
       <c r="H23" s="5">
-        <v>580480</v>
+        <v>698573</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="6">
-        <v>26.925000000000001</v>
+        <v>26.425000000000001</v>
       </c>
       <c r="C24" s="6">
-        <v>40.583333333333336</v>
+        <v>45.75</v>
       </c>
       <c r="D24" s="6">
-        <v>26.25</v>
+        <v>28.90625</v>
       </c>
       <c r="E24" s="7">
-        <v>3.102783203125</v>
+        <v>3.118896484375</v>
       </c>
       <c r="F24" s="7">
-        <v>10.691650390625</v>
+        <v>13.86669921875</v>
       </c>
       <c r="G24" s="7">
-        <v>13.79443359375</v>
+        <v>16.985595703125</v>
       </c>
       <c r="H24" s="5">
-        <v>595854</v>
+        <v>630718</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="6">
-        <v>26.55</v>
+        <v>25.5</v>
       </c>
       <c r="C25" s="6">
-        <v>42.541666666666664</v>
+        <v>39.541666666666664</v>
       </c>
       <c r="D25" s="6">
-        <v>26.1875</v>
+        <v>29.875</v>
       </c>
       <c r="E25" s="7">
-        <v>4.114501953125</v>
+        <v>4.00634765625</v>
       </c>
       <c r="F25" s="7">
-        <v>13.299560546875</v>
+        <v>12.248046875</v>
       </c>
       <c r="G25" s="7">
-        <v>17.4140625</v>
+        <v>16.25439453125</v>
       </c>
       <c r="H25" s="5">
-        <v>591366</v>
+        <v>580480</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6">
-        <v>26.324999999999999</v>
+        <v>26.925000000000001</v>
       </c>
       <c r="C26" s="6">
-        <v>42.458333333333336</v>
+        <v>40.583333333333336</v>
       </c>
       <c r="D26" s="6">
-        <v>26.125</v>
+        <v>26.25</v>
       </c>
       <c r="E26" s="7">
-        <v>4.0283203125</v>
+        <v>3.102783203125</v>
       </c>
       <c r="F26" s="7">
-        <v>13.634521484375</v>
+        <v>10.691650390625</v>
       </c>
       <c r="G26" s="7">
-        <v>17.662841796875</v>
+        <v>13.79443359375</v>
       </c>
       <c r="H26" s="5">
-        <v>598118</v>
+        <v>595854</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" s="6">
-        <v>26.875</v>
+        <v>26.55</v>
       </c>
       <c r="C27" s="6">
-        <v>47.083333333333336</v>
+        <v>42.541666666666664</v>
       </c>
       <c r="D27" s="6">
-        <v>28.75</v>
+        <v>26.1875</v>
       </c>
       <c r="E27" s="7">
-        <v>2.855224609375</v>
+        <v>4.114501953125</v>
       </c>
       <c r="F27" s="7">
-        <v>11.830078125</v>
+        <v>13.299560546875</v>
       </c>
       <c r="G27" s="7">
-        <v>14.685302734375</v>
+        <v>17.4140625</v>
       </c>
       <c r="H27" s="5">
-        <v>638878</v>
+        <v>591366</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="6">
+        <v>26.324999999999999</v>
+      </c>
+      <c r="C28" s="6">
+        <v>42.458333333333336</v>
+      </c>
+      <c r="D28" s="6">
         <v>26.125</v>
       </c>
-      <c r="C28" s="6">
-        <v>47</v>
-      </c>
-      <c r="D28" s="6">
-        <v>28.34375</v>
-      </c>
       <c r="E28" s="7">
-        <v>3.68798828125</v>
+        <v>4.0283203125</v>
       </c>
       <c r="F28" s="7">
-        <v>13.38427734375</v>
+        <v>13.634521484375</v>
       </c>
       <c r="G28" s="7">
-        <v>17.072265625</v>
+        <v>17.662841796875</v>
       </c>
       <c r="H28" s="5">
-        <v>624112</v>
+        <v>598118</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="6">
-        <v>25.024999999999999</v>
+        <v>26.875</v>
       </c>
       <c r="C29" s="6">
-        <v>42.916666666666664</v>
+        <v>47.083333333333336</v>
       </c>
       <c r="D29" s="6">
-        <v>27.8125</v>
+        <v>28.75</v>
       </c>
       <c r="E29" s="7">
-        <v>3.82763671875</v>
+        <v>2.855224609375</v>
       </c>
       <c r="F29" s="7">
-        <v>12.2890625</v>
+        <v>11.830078125</v>
       </c>
       <c r="G29" s="7">
-        <v>16.11669921875</v>
+        <v>14.685302734375</v>
       </c>
       <c r="H29" s="5">
-        <v>600254</v>
+        <v>638878</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6">
+        <v>26.125</v>
+      </c>
+      <c r="C30" s="6">
+        <v>47</v>
+      </c>
+      <c r="D30" s="6">
+        <v>28.34375</v>
+      </c>
+      <c r="E30" s="7">
+        <v>3.68798828125</v>
+      </c>
+      <c r="F30" s="7">
+        <v>13.38427734375</v>
+      </c>
+      <c r="G30" s="7">
+        <v>17.072265625</v>
+      </c>
+      <c r="H30" s="5">
+        <v>624112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="6">
+        <v>25.024999999999999</v>
+      </c>
+      <c r="C31" s="6">
+        <v>42.916666666666664</v>
+      </c>
+      <c r="D31" s="6">
+        <v>27.8125</v>
+      </c>
+      <c r="E31" s="7">
+        <v>3.82763671875</v>
+      </c>
+      <c r="F31" s="7">
+        <v>12.2890625</v>
+      </c>
+      <c r="G31" s="7">
+        <v>16.11669921875</v>
+      </c>
+      <c r="H31" s="5">
+        <v>600254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B32" s="6">
         <v>25.5</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C32" s="6">
         <v>45.666666666666664</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D32" s="6">
         <v>27.5625</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E32" s="7">
         <v>3.552734375</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F32" s="7">
         <v>12.682373046875</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G32" s="7">
         <v>16.235107421875</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H32" s="5">
         <v>619549</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify to add shcmg34bnk
</commit_message>
<xml_diff>
--- a/scripts/EPCCMGCutoverTemplate.xlsx
+++ b/scripts/EPCCMGCutoverTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>用户数</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,6 +213,10 @@
   </si>
   <si>
     <t>SHSAEGW37BNK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHSAEGW34BNK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -631,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1077,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1261,7 +1265,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1271,7 +1275,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1281,7 +1285,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1289,29 +1293,19 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="4">
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4">
         <v>43404.875</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>6</v>
@@ -1321,23 +1315,23 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="6">
-        <v>30.1</v>
-      </c>
-      <c r="C23" s="6">
-        <v>59.916666666666664</v>
-      </c>
-      <c r="D23" s="6">
-        <v>27.03125</v>
-      </c>
-      <c r="E23" s="7">
-        <v>4.182861328125</v>
-      </c>
-      <c r="F23" s="7">
-        <v>15.127197265625</v>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G23" s="7">
         <v>19.31005859375</v>
@@ -1348,22 +1342,22 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6">
-        <v>26.425000000000001</v>
+        <v>30.1</v>
       </c>
       <c r="C24" s="6">
-        <v>45.75</v>
+        <v>59.916666666666664</v>
       </c>
       <c r="D24" s="6">
-        <v>28.90625</v>
+        <v>27.03125</v>
       </c>
       <c r="E24" s="7">
-        <v>3.118896484375</v>
+        <v>4.182861328125</v>
       </c>
       <c r="F24" s="7">
-        <v>13.86669921875</v>
+        <v>15.127197265625</v>
       </c>
       <c r="G24" s="7">
         <v>16.985595703125</v>
@@ -1374,22 +1368,22 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="6">
-        <v>25.5</v>
+        <v>26.425000000000001</v>
       </c>
       <c r="C25" s="6">
-        <v>39.541666666666664</v>
+        <v>45.75</v>
       </c>
       <c r="D25" s="6">
-        <v>29.875</v>
+        <v>28.90625</v>
       </c>
       <c r="E25" s="7">
-        <v>4.00634765625</v>
+        <v>3.118896484375</v>
       </c>
       <c r="F25" s="7">
-        <v>12.248046875</v>
+        <v>13.86669921875</v>
       </c>
       <c r="G25" s="7">
         <v>16.25439453125</v>
@@ -1400,22 +1394,22 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="6">
-        <v>26.925000000000001</v>
+        <v>25.5</v>
       </c>
       <c r="C26" s="6">
-        <v>40.583333333333336</v>
+        <v>39.541666666666664</v>
       </c>
       <c r="D26" s="6">
-        <v>26.25</v>
+        <v>29.875</v>
       </c>
       <c r="E26" s="7">
-        <v>3.102783203125</v>
+        <v>4.00634765625</v>
       </c>
       <c r="F26" s="7">
-        <v>10.691650390625</v>
+        <v>12.248046875</v>
       </c>
       <c r="G26" s="7">
         <v>13.79443359375</v>
@@ -1426,22 +1420,22 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="6">
-        <v>26.55</v>
+        <v>26.925000000000001</v>
       </c>
       <c r="C27" s="6">
-        <v>42.541666666666664</v>
+        <v>40.583333333333336</v>
       </c>
       <c r="D27" s="6">
-        <v>26.1875</v>
+        <v>26.25</v>
       </c>
       <c r="E27" s="7">
-        <v>4.114501953125</v>
+        <v>3.102783203125</v>
       </c>
       <c r="F27" s="7">
-        <v>13.299560546875</v>
+        <v>10.691650390625</v>
       </c>
       <c r="G27" s="7">
         <v>17.4140625</v>
@@ -1452,22 +1446,22 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="6">
-        <v>26.324999999999999</v>
+        <v>26.55</v>
       </c>
       <c r="C28" s="6">
-        <v>42.458333333333336</v>
+        <v>42.541666666666664</v>
       </c>
       <c r="D28" s="6">
-        <v>26.125</v>
+        <v>26.1875</v>
       </c>
       <c r="E28" s="7">
-        <v>4.0283203125</v>
+        <v>4.114501953125</v>
       </c>
       <c r="F28" s="7">
-        <v>13.634521484375</v>
+        <v>13.299560546875</v>
       </c>
       <c r="G28" s="7">
         <v>17.662841796875</v>
@@ -1478,22 +1472,22 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="6">
-        <v>26.875</v>
+        <v>26.324999999999999</v>
       </c>
       <c r="C29" s="6">
-        <v>47.083333333333336</v>
+        <v>42.458333333333336</v>
       </c>
       <c r="D29" s="6">
-        <v>28.75</v>
+        <v>26.125</v>
       </c>
       <c r="E29" s="7">
-        <v>2.855224609375</v>
+        <v>4.0283203125</v>
       </c>
       <c r="F29" s="7">
-        <v>11.830078125</v>
+        <v>13.634521484375</v>
       </c>
       <c r="G29" s="7">
         <v>14.685302734375</v>
@@ -1504,22 +1498,22 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="6">
-        <v>26.125</v>
+        <v>26.875</v>
       </c>
       <c r="C30" s="6">
-        <v>47</v>
+        <v>47.083333333333336</v>
       </c>
       <c r="D30" s="6">
-        <v>28.34375</v>
+        <v>28.75</v>
       </c>
       <c r="E30" s="7">
-        <v>3.68798828125</v>
+        <v>2.855224609375</v>
       </c>
       <c r="F30" s="7">
-        <v>13.38427734375</v>
+        <v>11.830078125</v>
       </c>
       <c r="G30" s="7">
         <v>17.072265625</v>
@@ -1530,22 +1524,22 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="6">
-        <v>25.024999999999999</v>
+        <v>26.125</v>
       </c>
       <c r="C31" s="6">
-        <v>42.916666666666664</v>
+        <v>47</v>
       </c>
       <c r="D31" s="6">
-        <v>27.8125</v>
+        <v>28.34375</v>
       </c>
       <c r="E31" s="7">
-        <v>3.82763671875</v>
+        <v>3.68798828125</v>
       </c>
       <c r="F31" s="7">
-        <v>12.2890625</v>
+        <v>13.38427734375</v>
       </c>
       <c r="G31" s="7">
         <v>16.11669921875</v>
@@ -1556,22 +1550,22 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="6">
-        <v>25.5</v>
+        <v>25.024999999999999</v>
       </c>
       <c r="C32" s="6">
-        <v>45.666666666666664</v>
+        <v>42.916666666666664</v>
       </c>
       <c r="D32" s="6">
-        <v>27.5625</v>
+        <v>27.8125</v>
       </c>
       <c r="E32" s="7">
-        <v>3.552734375</v>
+        <v>3.82763671875</v>
       </c>
       <c r="F32" s="7">
-        <v>12.682373046875</v>
+        <v>12.2890625</v>
       </c>
       <c r="G32" s="7">
         <v>16.235107421875</v>
@@ -1580,43 +1574,63 @@
         <v>619549</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="6">
+        <v>25.5</v>
+      </c>
+      <c r="C33" s="6">
+        <v>45.666666666666664</v>
+      </c>
+      <c r="D33" s="6">
+        <v>27.5625</v>
+      </c>
+      <c r="E33" s="7">
+        <v>3.552734375</v>
+      </c>
+      <c r="F33" s="7">
+        <v>12.682373046875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>